<commit_message>
Update Sound classification folder Gurbuz code
update past results
</commit_message>
<xml_diff>
--- a/Results Documentation/Image Classification/Cifar100/DenseNet-BC-100/Results_densenet.xlsx
+++ b/Results Documentation/Image Classification/Cifar100/DenseNet-BC-100/Results_densenet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avichai\Desktop\Technion\Project_A\Deep-Neural-Networks-Calibration\Results Documentation\Image Classification\Cifar100\DenseNet-BC-100\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1145FCEC-B565-4541-AACD-83AC78E12B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9A97EC-F147-4345-8691-6090BDF6B181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27675" yWindow="1125" windowWidth="23610" windowHeight="11385" xr2:uid="{AA86E257-BB19-4E9E-8059-887006D9CF09}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="23610" windowHeight="11385" xr2:uid="{AA86E257-BB19-4E9E-8059-887006D9CF09}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
   <si>
     <t>Model</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Isotonic</t>
+  </si>
+  <si>
+    <t>n_bins=10</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -690,7 +693,9 @@
       <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="F7" s="2">
         <v>0.73068</v>
       </c>
@@ -717,7 +722,9 @@
       <c r="D8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="F8" s="2">
         <v>0.74968000000000001</v>
       </c>

</xml_diff>